<commit_message>
added new excel sheet and fixed a bug in Inventory Product service
</commit_message>
<xml_diff>
--- a/BackendProject/APIs.xlsx
+++ b/BackendProject/APIs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="124">
   <si>
     <t>method</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>{{baseUrl}}/api/v1/Auth/refresh</t>
+  </si>
+  <si>
+    <t>{"refreshToken":"token"}</t>
   </si>
   <si>
     <t>To blacklis the jwt token</t>
@@ -481,7 +484,6 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -498,6 +500,7 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -813,123 +816,127 @@
       <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="E6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="8"/>
     </row>
     <row r="7">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8">
-      <c r="B8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="E8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="F9" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10">
-      <c r="B10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="8"/>
     </row>
     <row r="11">
-      <c r="B11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>31</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -937,223 +944,223 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
-        <v>32</v>
+      <c r="A13" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F13" s="11"/>
     </row>
     <row r="14">
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="F14" s="11"/>
     </row>
     <row r="15">
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F15" s="11"/>
     </row>
     <row r="16">
       <c r="B16" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F17" s="4"/>
     </row>
     <row r="18">
       <c r="B18" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="F19" s="11"/>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F22" s="16"/>
     </row>
     <row r="23">
       <c r="B23" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F24" s="16"/>
     </row>
     <row r="25">
       <c r="B25" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F25" s="16"/>
     </row>
     <row r="26">
       <c r="B26" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F26" s="16"/>
     </row>
@@ -1162,127 +1169,127 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="6"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28">
       <c r="A28" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="D28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="F28" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="29">
-      <c r="B29" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="B29" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="9"/>
+      <c r="D29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="8"/>
     </row>
     <row r="30">
-      <c r="B30" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30" s="10" t="s">
+      <c r="B30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>69</v>
       </c>
+      <c r="D30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="31">
-      <c r="B31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="8" t="s">
+      <c r="B31" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F31" s="9"/>
+      <c r="D31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="8"/>
     </row>
     <row r="32">
-      <c r="B32" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="8" t="s">
+      <c r="B32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="9"/>
+      <c r="D32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="8"/>
     </row>
     <row r="33">
-      <c r="B33" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="8" t="s">
+      <c r="B33" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="9"/>
+      <c r="D33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="8"/>
     </row>
     <row r="34">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="6"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35">
       <c r="A35" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F35" s="21"/>
     </row>
@@ -1291,72 +1298,72 @@
         <v>6</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" s="19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C37" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C39" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" s="19" t="s">
         <v>87</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="24"/>
@@ -1366,234 +1373,234 @@
     </row>
     <row r="43">
       <c r="A43" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F44" s="16"/>
     </row>
     <row r="45">
       <c r="B45" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C46" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F46" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F49" s="14"/>
     </row>
     <row r="50">
       <c r="B50" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F55" s="14"/>
     </row>
     <row r="56">
       <c r="B56" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F56" s="14"/>
     </row>
@@ -1606,7 +1613,7 @@
     </row>
     <row r="58">
       <c r="A58" s="25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B58" s="26"/>
       <c r="C58" s="26"/>

</xml_diff>